<commit_message>
PST 4.0.0 and UM 1.0.0 Release
dub
</commit_message>
<xml_diff>
--- a/researchDocs/TEX/PST4UserManual/template/examples/extendedTerm/tableData.xlsx
+++ b/researchDocs/TEX/PST4UserManual/template/examples/extendedTerm/tableData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyth\source\repos\thadhaines\MT-Tech-SETO\researchDocs\TEX\one-offs\200806-ExtendedVersionComp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyth\source\repos\thadhaines\MT-Tech-SETO\researchDocs\TEX\PST4UserManual\template\examples\extendedTerm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
   <si>
     <t>Speed Up</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>3.1.1</t>
   </si>
   <si>
     <t>SETO</t>
@@ -397,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:W7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,19 +450,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -477,25 +474,25 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
         <v>15</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" t="s">
-        <v>16</v>
       </c>
       <c r="T3" t="s">
         <v>1</v>
@@ -508,8 +505,8 @@
       </c>
     </row>
     <row r="4" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="C4">
+        <v>3.1</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -557,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="S4">
-        <v>916.24</v>
+        <v>740.35</v>
       </c>
       <c r="T4" t="s">
         <v>1</v>
@@ -572,7 +569,7 @@
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -620,14 +617,14 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>250.82</v>
+        <v>284.37</v>
       </c>
       <c r="T5" t="s">
         <v>1</v>
       </c>
       <c r="U5" s="3">
         <f t="shared" ref="U5:U6" si="0">$S$4/S5</f>
-        <v>3.6529782314010046</v>
+        <v>2.6034743468017019</v>
       </c>
       <c r="V5" t="s">
         <v>3</v>
@@ -635,7 +632,7 @@
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -647,19 +644,19 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>2.6800000000000001E-4</v>
+        <v>1.36E-4</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>2.58E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <v>9315</v>
+        <v>17353</v>
       </c>
       <c r="L6" t="s">
         <v>1</v>
@@ -671,26 +668,26 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P6" t="s">
         <v>1</v>
       </c>
       <c r="Q6" s="2">
-        <v>17006</v>
+        <v>27243</v>
       </c>
       <c r="R6" t="s">
         <v>1</v>
       </c>
       <c r="S6">
-        <v>61.73</v>
+        <v>125.53</v>
       </c>
       <c r="T6" t="s">
         <v>1</v>
       </c>
       <c r="U6" s="3">
         <f t="shared" si="0"/>
-        <v>14.842702089745668</v>
+        <v>5.8977933561698404</v>
       </c>
       <c r="V6" t="s">
         <v>3</v>

</xml_diff>